<commit_message>
se arregla la creacion de OT
</commit_message>
<xml_diff>
--- a/CREAR OT SIN TAREA/datos excel/datos_OT.xlsx
+++ b/CREAR OT SIN TAREA/datos excel/datos_OT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eruhern\Documents\UiPath\CREAR OT SIN TAREA\datos excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C3DEB6-8441-4582-BF57-AF5E1781C7C4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C845F9-778C-41F8-9A86-2069518B4B36}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="-110" windowWidth="19420" windowHeight="14980" activeTab="1" xr2:uid="{8B51D6BE-9F50-4663-859D-D701AB2BE83D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{8B51D6BE-9F50-4663-859D-D701AB2BE83D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>FECHA HORA INICIO</t>
   </si>
@@ -58,22 +58,49 @@
     <t>ID OT</t>
   </si>
   <si>
-    <t>MPI_ANUAL_01-20_LETICIA NORTE (REMOTO)</t>
-  </si>
-  <si>
-    <t>REDCOM01S26296</t>
-  </si>
-  <si>
-    <t>MPI_SEMESTRAL_01-20_SAN JOSE DEL GUAVIARE AEROPUERTO</t>
-  </si>
-  <si>
-    <t>MLE_TGUV_520632</t>
-  </si>
-  <si>
-    <t>S26296</t>
-  </si>
-  <si>
-    <t>S26669</t>
+    <t>UL088</t>
+  </si>
+  <si>
+    <t>S27059</t>
+  </si>
+  <si>
+    <t>MPI_ANUAL_01-20_UNILEVER</t>
+  </si>
+  <si>
+    <t>REDCOM01S26550</t>
+  </si>
+  <si>
+    <t>MPI_ANUAL_01-20_ESTRUMENTAL</t>
+  </si>
+  <si>
+    <t>REDCOM01S26551</t>
+  </si>
+  <si>
+    <t>MPI_ANUAL_01-20_JARAMILLO MORA</t>
+  </si>
+  <si>
+    <t>MLL_TCAL_540681_024</t>
+  </si>
+  <si>
+    <t>MPI_ANUAL_01-20_PRONAVICOLA MEDIACANOA</t>
+  </si>
+  <si>
+    <t>UL9907_METROCELDA_PRONAVICOLA_MEDIOCANOA_7</t>
+  </si>
+  <si>
+    <t>MPI_SEMESTRAL_01-20_FLORA INDUSTRIAL (TRASLADO)</t>
+  </si>
+  <si>
+    <t>S26550</t>
+  </si>
+  <si>
+    <t>S26551</t>
+  </si>
+  <si>
+    <t>S25809</t>
+  </si>
+  <si>
+    <t>S26909</t>
   </si>
 </sst>
 </file>
@@ -535,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BEBE62-703C-4EDF-9FCC-A1DE376903C0}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -569,10 +596,10 @@
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="6"/>
     </row>
@@ -580,32 +607,44 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -712,6 +751,293 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="6"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="6"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="6"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="6"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="6"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="6"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="6"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -721,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B0DE604-C69A-41D3-BF4A-A25B2D89289E}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -749,30 +1075,72 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2">
-        <v>5178139</v>
+        <v>5182432</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
       <c r="C3">
-        <v>5178140</v>
+        <v>5182433</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>5182434</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>5182435</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>5182436</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>